<commit_message>
added functionality to pick best lot
</commit_message>
<xml_diff>
--- a/excel_data/2019_data/Win19_wk1_B.xlsx
+++ b/excel_data/2019_data/Win19_wk1_B.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016A7393-BB25-44F6-89C5-EB2EA0FF9DBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37643A7-C89D-4C01-B213-297DD0205ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{DC50A188-847D-4FC8-A023-AF284756115F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <r>
       <rPr>
@@ -517,82 +517,6 @@
   </si>
   <si>
     <t>Hopkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-59</t>
   </si>
   <si>
     <t>Pangea</t>
@@ -1292,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC7B1AD-A214-4418-B8A6-0A4B929B12DE}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1789,70 +1713,70 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="28.8">
+    <row r="8" spans="1:23">
       <c r="A8" s="62" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="42">
         <v>328</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="4">
+        <v>226</v>
+      </c>
+      <c r="E8" s="11">
+        <v>135</v>
+      </c>
+      <c r="F8" s="12">
+        <v>105</v>
+      </c>
+      <c r="G8" s="12">
+        <v>107</v>
+      </c>
+      <c r="H8" s="4">
+        <v>244</v>
+      </c>
+      <c r="I8" s="11">
+        <v>43</v>
+      </c>
+      <c r="J8" s="12">
+        <v>34</v>
+      </c>
+      <c r="K8" s="12">
+        <v>39</v>
+      </c>
+      <c r="L8" s="4">
+        <v>248</v>
+      </c>
+      <c r="M8" s="11">
         <v>64</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>81</v>
+      <c r="N8" s="12">
+        <v>19</v>
+      </c>
+      <c r="O8" s="13">
+        <v>21</v>
+      </c>
+      <c r="P8" s="4">
+        <v>214</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>108</v>
+      </c>
+      <c r="R8" s="12">
+        <v>20</v>
+      </c>
+      <c r="S8" s="12">
+        <v>28</v>
+      </c>
+      <c r="T8" s="4">
+        <v>257</v>
+      </c>
+      <c r="U8" s="11">
+        <v>187</v>
+      </c>
+      <c r="V8" s="11">
+        <v>59</v>
       </c>
       <c r="W8" s="11">
         <v>39</v>

</xml_diff>